<commit_message>
Made a smaller database to get away from size errors
</commit_message>
<xml_diff>
--- a/Civ V Unit Database.xlsx
+++ b/Civ V Unit Database.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="344">
   <si>
     <t>Unit</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>(None)</t>
+    <t>None</t>
   </si>
   <si>
     <t>Settler</t>
@@ -92,7 +92,7 @@
     <t>Bronze Working</t>
   </si>
   <si>
-    <t>Gains +50% bonus vs. Mounted</t>
+    <t>Gains plus 50 percent bonus vs. Mounted</t>
   </si>
   <si>
     <t>Chariot Archer</t>
@@ -131,7 +131,7 @@
     <t>Special</t>
   </si>
   <si>
-    <t>Has +25% bonus to nearby units; can build Citadel</t>
+    <t>Has plus 25 percent bonus to nearby units; can build Citadel</t>
   </si>
   <si>
     <t>Great Scientist</t>
@@ -182,7 +182,7 @@
     <t>Great Admiral</t>
   </si>
   <si>
-    <t>Gives +15% combat bonus, can heal nearby naval units</t>
+    <t>Gives plus 15 percent combat bonus, can heal nearby naval units</t>
   </si>
   <si>
     <t>Caravan</t>
@@ -221,52 +221,49 @@
     <t>Pathfinder</t>
   </si>
   <si>
-    <t>Shoshone UU*; Native Tongue, ignores terrain cost</t>
+    <t>Shoshone UU; Native Tongue, ignores terrain cost</t>
   </si>
   <si>
     <t>Khan</t>
   </si>
   <si>
-    <t>(Great General)</t>
-  </si>
-  <si>
-    <t>Mongolian UU*; Heals adjacent units.</t>
+    <t>Mongolian UU; Heals adjacent units.</t>
   </si>
   <si>
     <t>Brute</t>
   </si>
   <si>
-    <t>Barbarian UU*</t>
+    <t>Barbarian UU</t>
   </si>
   <si>
     <t>Galley</t>
   </si>
   <si>
-    <t>Barbarian UU*; Cannot enter deep ocean</t>
+    <t>Barbarian UU; Cannot enter deep ocean</t>
   </si>
   <si>
     <t>Hand-Axe</t>
   </si>
   <si>
-    <t>Barbarian UU*; may not melee attack</t>
+    <t>Barbarian UU; may not melee attack</t>
   </si>
   <si>
     <t>Bowman</t>
   </si>
   <si>
-    <t>Babylonian UU*;</t>
+    <t>Babylonian UU;</t>
   </si>
   <si>
     <t>War Chariot</t>
   </si>
   <si>
-    <t>Egyptian UU*; no defensive bonuses, rough terrain penalty</t>
+    <t>Egyptian UU; no defensive bonuses, rough terrain penalty</t>
   </si>
   <si>
     <t>Hoplite</t>
   </si>
   <si>
-    <t>Greek UU*; +100% vs Mounted</t>
+    <t>Greek UU; plus 100 percent vs Mounted</t>
   </si>
   <si>
     <t>Phalanx</t>
@@ -275,55 +272,55 @@
     <t>Mining</t>
   </si>
   <si>
-    <t>Sumerian UU*; +100% vs Mounted</t>
+    <t>Sumerian UU; plus 100 percent vs Mounted</t>
   </si>
   <si>
     <t>Heavy Chariot</t>
   </si>
   <si>
-    <t>Hittite UU*; Shock I</t>
+    <t>Hittite UU; Shock I</t>
   </si>
   <si>
     <t>Immortal</t>
   </si>
   <si>
-    <t>Persian UU*; +100% vs Mounted, heals at double rate</t>
+    <t>Persian UU; plus 100 percent vs Mounted, heals at double rate</t>
   </si>
   <si>
     <t>Jaguar</t>
   </si>
   <si>
-    <t>Aztec UU*; +50% combat strength in Jungle, heals +2 on kill, Woodsman</t>
+    <t>Aztec UU; plus 50 percent combat strength in Jungle, heals plus 2 on kill, Woodsman</t>
   </si>
   <si>
     <t>War Elephant</t>
   </si>
   <si>
-    <t>Indian UU*, no defensive bonuses</t>
+    <t>Indian UU, no defensive bonuses</t>
   </si>
   <si>
     <t>Slinger</t>
   </si>
   <si>
-    <t>Inca UU*; Withdraw Before Melee</t>
+    <t>Inca UU; Withdraw Before Melee</t>
   </si>
   <si>
     <t>Maori Warrior</t>
   </si>
   <si>
-    <t>Polyneisan UU*; Reduces enemy strength 10%</t>
+    <t>Polyneisan UU; Reduces enemy strength 10 percent</t>
   </si>
   <si>
     <t>Atlatlist</t>
   </si>
   <si>
-    <t>Mayan UU*; May Not Melee Attack</t>
+    <t>Mayan UU; May Not Melee Attack</t>
   </si>
   <si>
     <t>Pictish Warrior</t>
   </si>
   <si>
-    <t>Celtic UU*; +Faith per kill, free pillage, 20% Foreign Lands Bonus,</t>
+    <t>Celtic UU; plus Faith per kill, free pillage, 20 percent Foreign Lands Bonus,</t>
   </si>
   <si>
     <t>Battering Ram</t>
@@ -332,25 +329,25 @@
     <t>Siege</t>
   </si>
   <si>
-    <t>Hun UU*; +300% vs cities, (None)1 sight, (None)33% on defense, Cover I, City Attack Only, No Defense Bonus</t>
+    <t>Hun UU; plus 300 percent vs cities, -1 sight, -33 percent on defense, Cover I, City Attack Only, No Defense Bonus</t>
   </si>
   <si>
     <t>Horse Archer</t>
   </si>
   <si>
-    <t>Hun UU*; Accuracy I</t>
+    <t>Hun UU; Accuracy I</t>
   </si>
   <si>
     <t>Quinquereme</t>
   </si>
   <si>
-    <t>Carthage UU*; coast only</t>
+    <t>Carthage UU; coast only</t>
   </si>
   <si>
     <t>Dromon</t>
   </si>
   <si>
-    <t>Byzantine UU*; +50% vs naval, coast only</t>
+    <t>Byzantine UU; plus 50 percent vs naval, coast only</t>
   </si>
   <si>
     <t>Siege Tower</t>
@@ -359,7 +356,7 @@
     <t>Mathematics</t>
   </si>
   <si>
-    <t>Assyrian UU*; Sapper, +200% vs Cities, Cover I, +1 Sight, City attack only</t>
+    <t>Assyrian UU; Sapper, plus 200 percent vs Cities, Cover I, plus 1 Sight, City attack only</t>
   </si>
   <si>
     <t>African Forest Elephant</t>
@@ -368,7 +365,7 @@
     <t>Horseback Riding</t>
   </si>
   <si>
-    <t>Carthage UU*; Feared Elephant, Great Generals II, Can Move After Attacking, -33% vs. Cities, No Defensive Bonus</t>
+    <t>Carthage UU; Feared Elephant, Great Generals II, Can Move After Attacking, -33 percent vs. Cities, No Defensive Bonus</t>
   </si>
   <si>
     <t>Swordsman</t>
@@ -380,7 +377,7 @@
     <t>Horseman</t>
   </si>
   <si>
-    <t>Can move after attacking, no defensive bonuses, -33% vs cities</t>
+    <t>Can move after attacking, no defensive bonuses, -33 percent vs cities</t>
   </si>
   <si>
     <t>Composite Bowman</t>
@@ -392,43 +389,43 @@
     <t>Catapult</t>
   </si>
   <si>
-    <t>Must set up to fire; +200% vs Cities, -1 vision, no defensive bonuses</t>
+    <t>Must set up to fire; plus 200 percent vs Cities, -1 vision, no defensive bonuses</t>
   </si>
   <si>
     <t>Companion Cavalry</t>
   </si>
   <si>
-    <t>Greek UU*; can move after attack, Great Generals I, no defensive bonuses, -33% vs. Cities</t>
+    <t>Greek UU; can move after attack, Great Generals I, no defensive bonuses, -33 percent vs. Cities</t>
   </si>
   <si>
     <t>Legion</t>
   </si>
   <si>
-    <t>Roman UU*; Can build forts and roads.</t>
+    <t>Roman UU; Can build forts and roads.</t>
   </si>
   <si>
     <t>Ballista</t>
   </si>
   <si>
-    <t>Roman UU*; Must set up to fire; +200% vs Cities, -1 vision, no defensive bonuses</t>
+    <t>Roman UU; Must set up to fire; plus 200 percent vs Cities, -1 vision, no defensive bonuses</t>
   </si>
   <si>
     <t>Cataphract</t>
   </si>
   <si>
-    <t>Byzantine UU*; Can Move After Attacking, -25% vs. Cities</t>
+    <t>Byzantine UU; Can Move After Attacking, -25 percent vs. Cities</t>
   </si>
   <si>
     <t>Mohawk Warrior</t>
   </si>
   <si>
-    <t>Iroquois UU*; +50% combat strength in Forest/Jungle</t>
+    <t>Iroquois UU; plus 50 percent combat strength in Forest/Jungle</t>
   </si>
   <si>
     <t>Kris Swordsman</t>
   </si>
   <si>
-    <t>Indonesian UU*; Mystic Blade</t>
+    <t>Indonesian UU; Mystic Blade</t>
   </si>
   <si>
     <t>Pikeman</t>
@@ -437,7 +434,7 @@
     <t>Civil Service</t>
   </si>
   <si>
-    <t>Has +100% bonus vs. Mounted</t>
+    <t>Has plus 100 percent bonus vs. Mounted</t>
   </si>
   <si>
     <t>Crossbowman</t>
@@ -458,7 +455,7 @@
     <t>Chivalry</t>
   </si>
   <si>
-    <t>Can move after attacking, no defensive bonuses, -33% vs. Cities</t>
+    <t>Can move after attacking, no defensive bonuses, -33 percent vs. Cities</t>
   </si>
   <si>
     <t>Trebuchet</t>
@@ -470,73 +467,73 @@
     <t>Landsknecht</t>
   </si>
   <si>
-    <t>Has +50% vs Mounted, Free Pillage, Double Plunder, Can only be acquired through Commerce</t>
+    <t>Has plus 50 percent vs Mounted, Free Pillage, Double Plunder, Can only be acquired through Commerce</t>
   </si>
   <si>
     <t>Mandekalu Cavalry</t>
   </si>
   <si>
-    <t>Songhai UU*; can move after attacking, no defensive bonuses</t>
+    <t>Songhai UU; can move after attacking, no defensive bonuses</t>
   </si>
   <si>
     <t>Camel Archer</t>
   </si>
   <si>
-    <t>Arab UU*; Can Move After Attacking, no defensive bonsues</t>
+    <t>Arab UU; Can Move After Attacking, no defensive bonsues</t>
   </si>
   <si>
     <t>Keshik</t>
   </si>
   <si>
-    <t>Mongolian UU*; Great Generals I, Quick Study, can move after attacking, no defensive bonuses</t>
+    <t>Mongolian UU; Great Generals I, Quick Study, can move after attacking, no defensive bonuses</t>
   </si>
   <si>
     <t>Samurai</t>
   </si>
   <si>
-    <t>Japanese UU*; Shock I; Great Generals II; Can build Fishing Boats</t>
+    <t>Japanese UU; Shock I; Great Generals II; Can build Fishing Boats</t>
   </si>
   <si>
     <t>Longbowman</t>
   </si>
   <si>
-    <t>English UU*; May Not Melee Attack</t>
+    <t>English UU; May Not Melee Attack</t>
   </si>
   <si>
     <t>Chu-Ko-Nu</t>
   </si>
   <si>
-    <t>Chinese UU*; May Attack Twice</t>
-  </si>
-  <si>
-    <t>Naresuan's Elephant</t>
-  </si>
-  <si>
-    <t>Siamese UU*; +50% vs Mounted, can move after attacking, no defensive bonuses, -33% vs. Cities</t>
+    <t>Chinese UU; May Attack Twice</t>
+  </si>
+  <si>
+    <t>Naresuans Elephant</t>
+  </si>
+  <si>
+    <t>Siamese UU; plus 50 percent vs Mounted, can move after attacking, no defensive bonuses, -33 percent vs. Cities</t>
   </si>
   <si>
     <t>Berserker</t>
   </si>
   <si>
-    <t>Denmark UU*; Amphibious</t>
+    <t>Denmark UU; Amphibious</t>
   </si>
   <si>
     <t>Conquistador</t>
   </si>
   <si>
-    <t>Spanish UU*; no penalty vs. cities; +2 sight; Embarkation With Defense; can found cities</t>
-  </si>
-  <si>
-    <t>Hwach'a</t>
-  </si>
-  <si>
-    <t>Korean UU*; Must Set Up, No Defensive Bonuses</t>
+    <t>Spanish UU; no penalty vs. cities; plus 2 sight; Embarkation With Defense; can found cities</t>
+  </si>
+  <si>
+    <t>Hwacha</t>
+  </si>
+  <si>
+    <t>Korean UU; Must Set Up, No Defensive Bonuses</t>
   </si>
   <si>
     <t>Huscarl</t>
   </si>
   <si>
-    <t>Anglo Saxon UU*; +50% vs. Mounted, Cover I</t>
+    <t>Anglo Saxon UU; plus 50 percent vs. Mounted, Cover I</t>
   </si>
   <si>
     <t>Galleass</t>
@@ -551,13 +548,13 @@
     <t>Impi</t>
   </si>
   <si>
-    <t>Zulu UU*; Spear Throw, +50% vs Mounted</t>
+    <t>Zulu UU; Spear Throw, plus 50 percent vs Mounted</t>
   </si>
   <si>
     <t>Great Galleass</t>
   </si>
   <si>
-    <t>Venetian UU*; cannot enter deep ocean</t>
+    <t>Venetian UU; cannot enter deep ocean</t>
   </si>
   <si>
     <t>Musketman</t>
@@ -587,31 +584,31 @@
     <t>Astronomy</t>
   </si>
   <si>
-    <t>Has +1 Sight, Withdraw Before Melee</t>
+    <t>Has plus 1 Sight, Withdraw Before Melee</t>
   </si>
   <si>
     <t>Musketeer</t>
   </si>
   <si>
-    <t>French UU*</t>
+    <t>French UU</t>
   </si>
   <si>
     <t>Minuteman</t>
   </si>
   <si>
-    <t>American UU*; ignores terrain cost, Drill I</t>
+    <t>American UU; ignores terrain cost, Drill I</t>
   </si>
   <si>
     <t>Tercio</t>
   </si>
   <si>
-    <t>Spanish UU*; +50% vs Mounted</t>
+    <t>Spanish UU; plus 50 percent vs Mounted</t>
   </si>
   <si>
     <t>Turtle Ship</t>
   </si>
   <si>
-    <t>Korean UU*; Cannot Enter Deep Ocean</t>
+    <t>Korean UU; Cannot Enter Deep Ocean</t>
   </si>
   <si>
     <t>Frigate</t>
@@ -623,7 +620,7 @@
     <t>Ship of the Line</t>
   </si>
   <si>
-    <t>English UU*; +1 sight range</t>
+    <t>English UU; plus 1 sight range</t>
   </si>
   <si>
     <t>Privateer</t>
@@ -635,37 +632,37 @@
     <t>Sea Beggar</t>
   </si>
   <si>
-    <t>Dutch UU*; Prize Ships, Coastal Raider II, Supply</t>
+    <t>Dutch UU; Prize Ships, Coastal Raider II, Supply</t>
   </si>
   <si>
     <t>Hakkapeliitta</t>
   </si>
   <si>
-    <t>Swedish UU*; Formation I, +15% bonus when stacked with General, Can Move After Attacking, Transfer Movement to General</t>
+    <t>Swedish UU; Formation I, plus 15 percent bonus when stacked with General, Can Move After Attacking, Transfer Movement to General</t>
   </si>
   <si>
     <t>Sipahi</t>
   </si>
   <si>
-    <t>Ottoman UU* Formation I, +1 sight range, Can Move After Attacking, Free Pillage</t>
+    <t>Ottoman UU Formation I, plus 1 sight range, Can Move After Attacking, Free Pillage</t>
   </si>
   <si>
     <t>Janissary</t>
   </si>
   <si>
-    <t>Ottoman UU*; +25% strength when attacking; heals +50 if enemy destroyed</t>
+    <t>Ottoman UU; plus 25 percent strength when attacking; heals plus 50 if enemy destroyed</t>
   </si>
   <si>
     <t>Nau</t>
   </si>
   <si>
-    <t>Portguese UU*; Exotic Cargo, +1 Sight, Withdraw Before Melee</t>
+    <t>Portguese UU; Exotic Cargo, plus 1 Sight, Withdraw Before Melee</t>
   </si>
   <si>
     <t>Winged Hussar</t>
   </si>
   <si>
-    <t>Polish UU*; Heavy Charge, Shock I, Formation I, -33% vs Cities, no def. bonus, move after attack</t>
+    <t>Polish UU; Heavy Charge, Shock I, Formation I, -33 percent vs Cities, no def. bonus, move after attack</t>
   </si>
   <si>
     <t>Archaeologist</t>
@@ -689,7 +686,7 @@
     <t>Military Science</t>
   </si>
   <si>
-    <t>Can Move After Attacking, -33% vs Cities, No Defensive Bonuses</t>
+    <t>Can Move After Attacking, -33 percent vs Cities, No Defensive Bonuses</t>
   </si>
   <si>
     <t>Ironclad</t>
@@ -698,7 +695,7 @@
     <t>Steam Power</t>
   </si>
   <si>
-    <t>Has +33% vs Cities, Double Movement in Coast</t>
+    <t>Has plus 33 percent vs Cities, Double Movement in Coast</t>
   </si>
   <si>
     <t>Gatling Gun</t>
@@ -710,43 +707,43 @@
     <t>Cossack</t>
   </si>
   <si>
-    <t>Russian UU*; can move after attacking, +33% vs damaged units, -33% vs Cities, No Defensive Bonuses</t>
+    <t>Russian UU; can move after attacking, plus 33 percent vs damaged units, -33 percent vs Cities, No Defensive Bonuses</t>
   </si>
   <si>
     <t>Carolean</t>
   </si>
   <si>
-    <t>Swedish UU*; March</t>
+    <t>Swedish UU; March</t>
   </si>
   <si>
     <t>Norwegian Ski Infantry</t>
   </si>
   <si>
-    <t>Denmark UU*; bonuses on hills, snow, tundra</t>
+    <t>Denmark UU; bonuses on hills, snow, tundra</t>
   </si>
   <si>
     <t>Hussar</t>
   </si>
   <si>
-    <t>Austrian UU*; +1 Sight, +50% Flanking, Can Move After Attacking, -33% vs cities, No Defensive Bonses</t>
+    <t>Austrian UU; plus 1 Sight, plus 50 percent Flanking, Can Move After Attacking, -33 percent vs cities, No Defensive Bonses</t>
   </si>
   <si>
     <t>Mehal Sefari</t>
   </si>
   <si>
-    <t>Ethiopian UU*; Drill I, Near Capital Bonus</t>
+    <t>Ethiopian UU; Drill I, Near Capital Bonus</t>
   </si>
   <si>
     <t>Berber Cavalry</t>
   </si>
   <si>
-    <t>Moroccan UU*; bonus in Desert and friendly territory</t>
+    <t>Moroccan UU; bonus in Desert and friendly territory</t>
   </si>
   <si>
     <t>Comanche Riders</t>
   </si>
   <si>
-    <t>Shoshone UU*; +1 Move</t>
+    <t>Shoshone UU; plus 1 Move</t>
   </si>
   <si>
     <t>Machine Gun</t>
@@ -764,7 +761,7 @@
     <t>Flight</t>
   </si>
   <si>
-    <t>Interception (50), Air Sweep, Air Recon, +150% vs Bombers and Helicopters</t>
+    <t>Interception (50), Air Sweep, Air Recon, plus 150 percent vs Bombers and Helicopters</t>
   </si>
   <si>
     <t>Great War Bomber</t>
@@ -782,9 +779,6 @@
     <t>Combustion</t>
   </si>
   <si>
-    <t>(WWI Tank)</t>
-  </si>
-  <si>
     <t>Infantry</t>
   </si>
   <si>
@@ -797,7 +791,7 @@
     <t>Dynamite</t>
   </si>
   <si>
-    <t>Must set up to fire; +200% vs Cities, -1 vision, no defensive bonuses, Indirect Fire</t>
+    <t>Must set up to fire; plus 200 percent vs Cities, -1 vision, no defensive bonuses, Indirect Fire</t>
   </si>
   <si>
     <t>Destroyer</t>
@@ -806,7 +800,7 @@
     <t>Electricity</t>
   </si>
   <si>
-    <t>Has +3 sight range, +100% vs Submarines, Intercept, Indirect Fire</t>
+    <t>Has plus 3 sight range, plus 100 percent vs Submarines, Intercept, Indirect Fire</t>
   </si>
   <si>
     <t>Battleship</t>
@@ -824,13 +818,13 @@
     <t>Refrigeration</t>
   </si>
   <si>
-    <t>Invisible, Can See Submarines, May Enter Ice Tiles, +100 on attack</t>
+    <t>Invisible, Can See Submarines, May Enter Ice Tiles, plus 100 on attack</t>
   </si>
   <si>
     <t>Foreign Legion</t>
   </si>
   <si>
-    <t>Foreign Lands +20% Bonus</t>
+    <t>Foreign Lands plus 20 percent Bonus</t>
   </si>
   <si>
     <t>Anti-Tank Gun</t>
@@ -839,7 +833,7 @@
     <t>Combined Arms</t>
   </si>
   <si>
-    <t>Has +100% vs. Armor</t>
+    <t>Has plus 100 percent vs. Armor</t>
   </si>
   <si>
     <t>Anti-Aircraft Gun</t>
@@ -848,13 +842,13 @@
     <t>Radio</t>
   </si>
   <si>
-    <t>Interception(100), +150% vs. bombers &amp; helicopters</t>
+    <t>Interception(100), plus 150 percent vs. bombers &amp; helicopters</t>
   </si>
   <si>
     <t>Pracinha</t>
   </si>
   <si>
-    <t>Brazilian UU*; Golden Age from Victories</t>
+    <t>Brazilian UU; Golden Age from Victories</t>
   </si>
   <si>
     <t>Tank</t>
@@ -866,7 +860,7 @@
     <t>Fighter</t>
   </si>
   <si>
-    <t>Interception(100), Air Sweep, Recon, +150% vs Bombers &amp; Helicopters</t>
+    <t>Interception(100), Air Sweep, Recon, plus 150 percent vs Bombers &amp; Helicopters</t>
   </si>
   <si>
     <t>Bomber</t>
@@ -890,7 +884,7 @@
     <t>Penicillin</t>
   </si>
   <si>
-    <t>Amphibious, +1 Sight When Embarked, Double Embarked Defense</t>
+    <t>Amphibious, plus 1 Sight When Embarked, Double Embarked Defense</t>
   </si>
   <si>
     <t>Paratrooper</t>
@@ -902,19 +896,19 @@
     <t>Panzer</t>
   </si>
   <si>
-    <t>German UU*; can move after attack, No Defensive Bonuses</t>
+    <t>German UU; can move after attack, No Defensive Bonuses</t>
   </si>
   <si>
     <t>Zero</t>
   </si>
   <si>
-    <t>Japanese UU*; Interception(100), +33% vs Fighters, Recon, Air Sweep, +150 vs Bombers &amp; Helicopters</t>
+    <t>Japanese UU; Interception(100), plus 33 percent vs Fighters, Recon, Air Sweep, plus 150 vs Bombers &amp; Helicopters</t>
   </si>
   <si>
     <t>B-17</t>
   </si>
   <si>
-    <t>American UU*; Evasion, Melee 1</t>
+    <t>American UU; Evasion, Melee 1</t>
   </si>
   <si>
     <t>Atomic Bomb</t>
@@ -938,7 +932,7 @@
     <t>Rocketry</t>
   </si>
   <si>
-    <t>All Tile Cost 1, Hovering Unit, +100 vs Tanks, No Defensive Bonuses, Can't Capture Cities</t>
+    <t>All Tile Cost 1, Hovering Unit, plus 100 vs Tanks, No Defensive Bonuses, Cannot Capture Cities</t>
   </si>
   <si>
     <t>Rocket Artillery</t>
@@ -950,7 +944,7 @@
     <t>Computers</t>
   </si>
   <si>
-    <t>Interception(100), +150% vs. Air</t>
+    <t>Interception(100), plus 150 percent vs. Air</t>
   </si>
   <si>
     <t>Jet Fighter</t>
@@ -959,7 +953,7 @@
     <t>Lasers</t>
   </si>
   <si>
-    <t>Interception(100), Recon, Air Sweep, +150 vs Bombers &amp; Helicopters</t>
+    <t>Interception(100), Recon, Air Sweep, plus 150 vs Bombers &amp; Helicopters</t>
   </si>
   <si>
     <t>Modern Armor</t>
@@ -1001,7 +995,7 @@
     <t>Nuclear Submarine</t>
   </si>
   <si>
-    <t>Can carry 2 missiles; +100 vs submarines; invisible, Can See Submarines, May Enter Ice Tiles</t>
+    <t>Can carry 2 missiles; plus 100 vs submarines; invisible, Can See Submarines, May Enter Ice Tiles</t>
   </si>
   <si>
     <t>Missile Cruiser</t>
@@ -1010,7 +1004,7 @@
     <t>Robotics</t>
   </si>
   <si>
-    <t>Can See Submarines, +100 vs Submarines, Can Carry 3 Cargo, Interception(100)</t>
+    <t>Can See Submarines, plus 100 vs Submarines, Can Carry 3 Cargo, Interception(100)</t>
   </si>
   <si>
     <t>XCOM Squad</t>
@@ -1167,7 +1161,7 @@
     <col customWidth="1" min="3" max="3" width="9.29"/>
     <col customWidth="1" min="4" max="4" width="17.0"/>
     <col customWidth="1" min="5" max="6" width="6.71"/>
-    <col customWidth="1" min="7" max="7" width="105.0"/>
+    <col customWidth="1" min="7" max="7" width="112.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1854,7 +1848,7 @@
         <v>38</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>10</v>
@@ -1863,7 +1857,7 @@
         <v>5.0</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1872,7 +1866,7 @@
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>8</v>
@@ -1890,7 +1884,7 @@
         <v>2.0</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1899,7 +1893,7 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>8</v>
@@ -1917,7 +1911,7 @@
         <v>3.0</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1926,7 +1920,7 @@
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>20</v>
@@ -1944,7 +1938,7 @@
         <v>2.0</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1953,7 +1947,7 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>20</v>
@@ -1971,7 +1965,7 @@
         <v>2.0</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1980,7 +1974,7 @@
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>20</v>
@@ -1998,7 +1992,7 @@
         <v>5.0</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -2007,7 +2001,7 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>8</v>
@@ -2025,7 +2019,7 @@
         <v>2.0</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -2034,7 +2028,7 @@
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>8</v>
@@ -2043,7 +2037,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E33" s="4">
         <v>56.0</v>
@@ -2052,7 +2046,7 @@
         <v>2.0</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -2061,7 +2055,7 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>20</v>
@@ -2079,7 +2073,7 @@
         <v>3.0</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2088,7 +2082,7 @@
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>8</v>
@@ -2106,7 +2100,7 @@
         <v>2.0</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -2115,7 +2109,7 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>8</v>
@@ -2133,7 +2127,7 @@
         <v>2.0</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -2142,7 +2136,7 @@
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>20</v>
@@ -2160,7 +2154,7 @@
         <v>3.0</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -2169,7 +2163,7 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>20</v>
@@ -2187,7 +2181,7 @@
         <v>2.0</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2196,7 +2190,7 @@
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>8</v>
@@ -2214,7 +2208,7 @@
         <v>2.0</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2223,7 +2217,7 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>20</v>
@@ -2241,7 +2235,7 @@
         <v>2.0</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -2250,7 +2244,7 @@
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>8</v>
@@ -2268,7 +2262,7 @@
         <v>2.0</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
@@ -2277,13 +2271,13 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>25</v>
@@ -2295,7 +2289,7 @@
         <v>2.0</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
@@ -2304,7 +2298,7 @@
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>20</v>
@@ -2322,7 +2316,7 @@
         <v>4.0</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -2331,7 +2325,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>8</v>
@@ -2349,7 +2343,7 @@
         <v>4.0</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -2358,7 +2352,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>20</v>
@@ -2376,7 +2370,7 @@
         <v>4.0</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
@@ -2385,16 +2379,16 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="E46" s="4">
         <v>75.0</v>
@@ -2403,7 +2397,7 @@
         <v>2.0</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
@@ -2412,7 +2406,7 @@
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>8</v>
@@ -2421,7 +2415,7 @@
         <v>28</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E47" s="4">
         <v>100.0</v>
@@ -2430,7 +2424,7 @@
         <v>3.0</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
@@ -2439,7 +2433,7 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>8</v>
@@ -2448,7 +2442,7 @@
         <v>9</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E48" s="4">
         <v>75.0</v>
@@ -2464,7 +2458,7 @@
     </row>
     <row r="49">
       <c r="A49" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>8</v>
@@ -2473,7 +2467,7 @@
         <v>28</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E49" s="4">
         <v>75.0</v>
@@ -2482,7 +2476,7 @@
         <v>4.0</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
@@ -2491,7 +2485,7 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>20</v>
@@ -2500,7 +2494,7 @@
         <v>9</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E50" s="4">
         <v>75.0</v>
@@ -2518,16 +2512,16 @@
     </row>
     <row r="51">
       <c r="A51" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E51" s="4">
         <v>75.0</v>
@@ -2536,7 +2530,7 @@
         <v>2.0</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
@@ -2545,7 +2539,7 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>8</v>
@@ -2554,7 +2548,7 @@
         <v>28</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E52" s="4">
         <v>75.0</v>
@@ -2563,7 +2557,7 @@
         <v>5.0</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
@@ -2572,7 +2566,7 @@
     </row>
     <row r="53">
       <c r="A53" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>8</v>
@@ -2581,7 +2575,7 @@
         <v>9</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E53" s="4">
         <v>75.0</v>
@@ -2590,7 +2584,7 @@
         <v>2.0</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
@@ -2599,16 +2593,16 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E54" s="4">
         <v>75.0</v>
@@ -2617,7 +2611,7 @@
         <v>2.0</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
@@ -2626,7 +2620,7 @@
     </row>
     <row r="55">
       <c r="A55" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>8</v>
@@ -2635,7 +2629,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E55" s="4">
         <v>75.0</v>
@@ -2644,7 +2638,7 @@
         <v>3.0</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -2653,7 +2647,7 @@
     </row>
     <row r="56">
       <c r="A56" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>8</v>
@@ -2662,7 +2656,7 @@
         <v>9</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E56" s="4">
         <v>75.0</v>
@@ -2671,7 +2665,7 @@
         <v>2.0</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
@@ -2680,7 +2674,7 @@
     </row>
     <row r="57">
       <c r="A57" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>8</v>
@@ -2689,7 +2683,7 @@
         <v>9</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E57" s="4">
         <v>75.0</v>
@@ -2698,7 +2692,7 @@
         <v>2.0</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
@@ -2707,7 +2701,7 @@
     </row>
     <row r="58">
       <c r="A58" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>8</v>
@@ -2716,7 +2710,7 @@
         <v>9</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E58" s="4">
         <v>90.0</v>
@@ -2725,7 +2719,7 @@
         <v>2.0</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
@@ -2734,7 +2728,7 @@
     </row>
     <row r="59">
       <c r="A59" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>20</v>
@@ -2743,7 +2737,7 @@
         <v>9</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E59" s="4">
         <v>120.0</v>
@@ -2761,7 +2755,7 @@
     </row>
     <row r="60">
       <c r="A60" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>8</v>
@@ -2770,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E60" s="4">
         <v>120.0</v>
@@ -2786,7 +2780,7 @@
     </row>
     <row r="61">
       <c r="A61" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>8</v>
@@ -2795,7 +2789,7 @@
         <v>9</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E61" s="4">
         <v>120.0</v>
@@ -2804,7 +2798,7 @@
         <v>4.0</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
@@ -2813,16 +2807,16 @@
     </row>
     <row r="62">
       <c r="A62" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E62" s="4">
         <v>120.0</v>
@@ -2831,7 +2825,7 @@
         <v>2.0</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -2840,7 +2834,7 @@
     </row>
     <row r="63">
       <c r="A63" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>8</v>
@@ -2849,7 +2843,7 @@
         <v>38</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E63" s="4">
         <v>45.0</v>
@@ -2858,7 +2852,7 @@
         <v>2.0</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
@@ -2867,7 +2861,7 @@
     </row>
     <row r="64">
       <c r="A64" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>8</v>
@@ -2876,7 +2870,7 @@
         <v>9</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E64" s="4">
         <v>120.0</v>
@@ -2885,7 +2879,7 @@
         <v>4.0</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
@@ -2894,7 +2888,7 @@
     </row>
     <row r="65">
       <c r="A65" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>20</v>
@@ -2903,7 +2897,7 @@
         <v>28</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E65" s="4">
         <v>120.0</v>
@@ -2912,7 +2906,7 @@
         <v>4.0</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
@@ -2921,7 +2915,7 @@
     </row>
     <row r="66">
       <c r="A66" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>20</v>
@@ -2930,7 +2924,7 @@
         <v>28</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E66" s="4">
         <v>165.0</v>
@@ -2939,7 +2933,7 @@
         <v>5.0</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
@@ -2948,7 +2942,7 @@
     </row>
     <row r="67">
       <c r="A67" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>8</v>
@@ -2957,7 +2951,7 @@
         <v>9</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E67" s="4">
         <v>120.0</v>
@@ -2966,7 +2960,7 @@
         <v>2.0</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H67" s="3"/>
       <c r="I67" s="3"/>
@@ -2975,7 +2969,7 @@
     </row>
     <row r="68">
       <c r="A68" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>20</v>
@@ -2984,7 +2978,7 @@
         <v>9</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E68" s="4">
         <v>120.0</v>
@@ -2993,7 +2987,7 @@
         <v>2.0</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H68" s="3"/>
       <c r="I68" s="3"/>
@@ -3002,7 +2996,7 @@
     </row>
     <row r="69">
       <c r="A69" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>20</v>
@@ -3011,7 +3005,7 @@
         <v>9</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E69" s="4">
         <v>120.0</v>
@@ -3020,7 +3014,7 @@
         <v>2.0</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H69" s="3"/>
       <c r="I69" s="3"/>
@@ -3029,7 +3023,7 @@
     </row>
     <row r="70">
       <c r="A70" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>20</v>
@@ -3038,7 +3032,7 @@
         <v>24</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E70" s="4">
         <v>120.0</v>
@@ -3047,7 +3041,7 @@
         <v>3.0</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
@@ -3056,7 +3050,7 @@
     </row>
     <row r="71">
       <c r="A71" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>8</v>
@@ -3065,7 +3059,7 @@
         <v>9</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E71" s="4">
         <v>120.0</v>
@@ -3074,7 +3068,7 @@
         <v>3.0</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
@@ -3083,7 +3077,7 @@
     </row>
     <row r="72">
       <c r="A72" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>8</v>
@@ -3092,7 +3086,7 @@
         <v>9</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E72" s="4">
         <v>120.0</v>
@@ -3101,7 +3095,7 @@
         <v>4.0</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
@@ -3110,16 +3104,16 @@
     </row>
     <row r="73">
       <c r="A73" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E73" s="4">
         <v>120.0</v>
@@ -3128,7 +3122,7 @@
         <v>2.0</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
@@ -3137,7 +3131,7 @@
     </row>
     <row r="74">
       <c r="A74" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>8</v>
@@ -3146,7 +3140,7 @@
         <v>24</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E74" s="4">
         <v>110.0</v>
@@ -3155,7 +3149,7 @@
         <v>2.0</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -3164,7 +3158,7 @@
     </row>
     <row r="75">
       <c r="A75" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>20</v>
@@ -3173,7 +3167,7 @@
         <v>32</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E75" s="4">
         <v>100.0</v>
@@ -3182,7 +3176,7 @@
         <v>3.0</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
@@ -3191,7 +3185,7 @@
     </row>
     <row r="76">
       <c r="A76" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>8</v>
@@ -3200,7 +3194,7 @@
         <v>24</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E76" s="4">
         <v>90.0</v>
@@ -3209,7 +3203,7 @@
         <v>2.0</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
@@ -3218,7 +3212,7 @@
     </row>
     <row r="77">
       <c r="A77" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>8</v>
@@ -3227,7 +3221,7 @@
         <v>9</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E77" s="4">
         <v>110.0</v>
@@ -3236,7 +3230,7 @@
         <v>3.0</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
@@ -3245,7 +3239,7 @@
     </row>
     <row r="78">
       <c r="A78" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>8</v>
@@ -3254,7 +3248,7 @@
         <v>9</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E78" s="4">
         <v>150.0</v>
@@ -3270,7 +3264,7 @@
     </row>
     <row r="79">
       <c r="A79" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>8</v>
@@ -3279,7 +3273,7 @@
         <v>24</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E79" s="4">
         <v>185.0</v>
@@ -3288,7 +3282,7 @@
         <v>4.0</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
@@ -3297,16 +3291,16 @@
     </row>
     <row r="80">
       <c r="A80" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E80" s="4">
         <v>185.0</v>
@@ -3315,7 +3309,7 @@
         <v>2.0</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -3324,7 +3318,7 @@
     </row>
     <row r="81">
       <c r="A81" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>8</v>
@@ -3333,7 +3327,7 @@
         <v>17</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E81" s="4">
         <v>120.0</v>
@@ -3342,7 +3336,7 @@
         <v>4.0</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -3351,7 +3345,7 @@
     </row>
     <row r="82">
       <c r="A82" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>8</v>
@@ -3360,7 +3354,7 @@
         <v>9</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E82" s="4">
         <v>150.0</v>
@@ -3369,7 +3363,7 @@
         <v>2.0</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
@@ -3378,7 +3372,7 @@
     </row>
     <row r="83">
       <c r="A83" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>8</v>
@@ -3387,7 +3381,7 @@
         <v>9</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E83" s="4">
         <v>150.0</v>
@@ -3396,7 +3390,7 @@
         <v>2.0</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -3405,7 +3399,7 @@
     </row>
     <row r="84">
       <c r="A84" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>8</v>
@@ -3414,7 +3408,7 @@
         <v>9</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E84" s="4">
         <v>155.0</v>
@@ -3423,7 +3417,7 @@
         <v>2.0</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -3432,7 +3426,7 @@
     </row>
     <row r="85">
       <c r="A85" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>8</v>
@@ -3441,7 +3435,7 @@
         <v>32</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E85" s="4">
         <v>120.0</v>
@@ -3450,7 +3444,7 @@
         <v>4.0</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -3459,7 +3453,7 @@
     </row>
     <row r="86">
       <c r="A86" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>20</v>
@@ -3468,7 +3462,7 @@
         <v>32</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E86" s="4">
         <v>185.0</v>
@@ -3486,7 +3480,7 @@
     </row>
     <row r="87">
       <c r="A87" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>20</v>
@@ -3495,7 +3489,7 @@
         <v>32</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E87" s="4">
         <v>170.0</v>
@@ -3504,7 +3498,7 @@
         <v>7.0</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
@@ -3513,7 +3507,7 @@
     </row>
     <row r="88">
       <c r="A88" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>8</v>
@@ -3522,7 +3516,7 @@
         <v>32</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E88" s="4">
         <v>150.0</v>
@@ -3531,7 +3525,7 @@
         <v>5.0</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
@@ -3540,7 +3534,7 @@
     </row>
     <row r="89">
       <c r="A89" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>8</v>
@@ -3549,7 +3543,7 @@
         <v>32</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E89" s="4">
         <v>150.0</v>
@@ -3558,7 +3552,7 @@
         <v>5.0</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
@@ -3567,7 +3561,7 @@
     </row>
     <row r="90">
       <c r="A90" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>8</v>
@@ -3576,7 +3570,7 @@
         <v>28</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E90" s="4">
         <v>185.0</v>
@@ -3585,7 +3579,7 @@
         <v>4.0</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
@@ -3594,7 +3588,7 @@
     </row>
     <row r="91">
       <c r="A91" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>8</v>
@@ -3603,7 +3597,7 @@
         <v>28</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E91" s="4">
         <v>185.0</v>
@@ -3612,7 +3606,7 @@
         <v>5.0</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
@@ -3621,7 +3615,7 @@
     </row>
     <row r="92">
       <c r="A92" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>8</v>
@@ -3630,7 +3624,7 @@
         <v>9</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E92" s="4">
         <v>150.0</v>
@@ -3639,7 +3633,7 @@
         <v>2.0</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -3648,7 +3642,7 @@
     </row>
     <row r="93">
       <c r="A93" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>8</v>
@@ -3657,7 +3651,7 @@
         <v>32</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E93" s="4">
         <v>120.0</v>
@@ -3666,7 +3660,7 @@
         <v>5.0</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
@@ -3675,7 +3669,7 @@
     </row>
     <row r="94">
       <c r="A94" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>8</v>
@@ -3684,7 +3678,7 @@
         <v>28</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E94" s="4">
         <v>185.0</v>
@@ -3693,7 +3687,7 @@
         <v>5.0</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
@@ -3702,7 +3696,7 @@
     </row>
     <row r="95">
       <c r="A95" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>12</v>
@@ -3711,7 +3705,7 @@
         <v>12</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E95" s="4">
         <v>200.0</v>
@@ -3720,7 +3714,7 @@
         <v>4.0</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
@@ -3729,7 +3723,7 @@
     </row>
     <row r="96">
       <c r="A96" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>8</v>
@@ -3738,7 +3732,7 @@
         <v>9</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E96" s="4">
         <v>225.0</v>
@@ -3754,7 +3748,7 @@
     </row>
     <row r="97">
       <c r="A97" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>8</v>
@@ -3763,7 +3757,7 @@
         <v>28</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E97" s="4">
         <v>225.0</v>
@@ -3772,7 +3766,7 @@
         <v>4.0</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
@@ -3781,7 +3775,7 @@
     </row>
     <row r="98">
       <c r="A98" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>8</v>
@@ -3790,7 +3784,7 @@
         <v>32</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E98" s="4">
         <v>270.0</v>
@@ -3799,7 +3793,7 @@
         <v>3.0</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
@@ -3808,7 +3802,7 @@
     </row>
     <row r="99">
       <c r="A99" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>20</v>
@@ -3817,7 +3811,7 @@
         <v>9</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E99" s="4">
         <v>225.0</v>
@@ -3835,7 +3829,7 @@
     </row>
     <row r="100">
       <c r="A100" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B100" s="4" t="s">
         <v>8</v>
@@ -3844,7 +3838,7 @@
         <v>28</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E100" s="4">
         <v>225.0</v>
@@ -3853,7 +3847,7 @@
         <v>4.0</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
@@ -3862,7 +3856,7 @@
     </row>
     <row r="101">
       <c r="A101" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>8</v>
@@ -3871,7 +3865,7 @@
         <v>9</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E101" s="4">
         <v>225.0</v>
@@ -3880,7 +3874,7 @@
         <v>2.0</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
@@ -3889,7 +3883,7 @@
     </row>
     <row r="102">
       <c r="A102" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>8</v>
@@ -3898,7 +3892,7 @@
         <v>9</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E102" s="4">
         <v>220.0</v>
@@ -3907,7 +3901,7 @@
         <v>2.0</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
@@ -3916,7 +3910,7 @@
     </row>
     <row r="103">
       <c r="A103" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>8</v>
@@ -3925,7 +3919,7 @@
         <v>28</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E103" s="4">
         <v>225.0</v>
@@ -3934,7 +3928,7 @@
         <v>5.0</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
@@ -3943,7 +3937,7 @@
     </row>
     <row r="104">
       <c r="A104" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>8</v>
@@ -3952,7 +3946,7 @@
         <v>9</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E104" s="4">
         <v>200.0</v>
@@ -3961,7 +3955,7 @@
         <v>2.0</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
@@ -3970,7 +3964,7 @@
     </row>
     <row r="105">
       <c r="A105" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>8</v>
@@ -3979,7 +3973,7 @@
         <v>28</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E105" s="4">
         <v>225.0</v>
@@ -3988,7 +3982,7 @@
         <v>4.0</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
@@ -3997,7 +3991,7 @@
     </row>
     <row r="106">
       <c r="A106" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>8</v>
@@ -4006,7 +4000,7 @@
         <v>28</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E106" s="4">
         <v>200.0</v>
@@ -4015,7 +4009,7 @@
         <v>4.0</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
@@ -4024,7 +4018,7 @@
     </row>
     <row r="107">
       <c r="A107" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>20</v>
@@ -4033,7 +4027,7 @@
         <v>9</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E107" s="4">
         <v>350.0</v>
@@ -4051,16 +4045,16 @@
     </row>
     <row r="108">
       <c r="A108" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B108" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C108" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D108" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="E108" s="4">
         <v>325.0</v>
@@ -4069,7 +4063,7 @@
         <v>10</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
@@ -4078,16 +4072,16 @@
     </row>
     <row r="109">
       <c r="A109" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C109" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="E109" s="4">
         <v>325.0</v>
@@ -4103,7 +4097,7 @@
     </row>
     <row r="110">
       <c r="A110" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>8</v>
@@ -4112,7 +4106,7 @@
         <v>9</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E110" s="4">
         <v>320.0</v>
@@ -4128,7 +4122,7 @@
     </row>
     <row r="111">
       <c r="A111" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>8</v>
@@ -4137,7 +4131,7 @@
         <v>28</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E111" s="4">
         <v>350.0</v>
@@ -4145,9 +4139,7 @@
       <c r="F111" s="4">
         <v>4.0</v>
       </c>
-      <c r="G111" s="4" t="s">
-        <v>256</v>
-      </c>
+      <c r="G111" s="4"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
@@ -4155,7 +4147,7 @@
     </row>
     <row r="112">
       <c r="A112" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>8</v>
@@ -4164,7 +4156,7 @@
         <v>9</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E112" s="4">
         <v>320.0</v>
@@ -4180,16 +4172,16 @@
     </row>
     <row r="113">
       <c r="A113" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E113" s="4">
         <v>250.0</v>
@@ -4198,7 +4190,7 @@
         <v>2.0</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
@@ -4207,7 +4199,7 @@
     </row>
     <row r="114">
       <c r="A114" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>8</v>
@@ -4216,7 +4208,7 @@
         <v>32</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E114" s="4">
         <v>375.0</v>
@@ -4225,7 +4217,7 @@
         <v>6.0</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
@@ -4234,7 +4226,7 @@
     </row>
     <row r="115">
       <c r="A115" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>20</v>
@@ -4243,7 +4235,7 @@
         <v>32</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E115" s="4">
         <v>375.0</v>
@@ -4252,7 +4244,7 @@
         <v>3.0</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
@@ -4261,7 +4253,7 @@
     </row>
     <row r="116">
       <c r="A116" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>20</v>
@@ -4270,7 +4262,7 @@
         <v>32</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E116" s="4">
         <v>375.0</v>
@@ -4279,7 +4271,7 @@
         <v>5.0</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
@@ -4288,7 +4280,7 @@
     </row>
     <row r="117">
       <c r="A117" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>8</v>
@@ -4297,7 +4289,7 @@
         <v>9</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E117" s="4">
         <v>320.0</v>
@@ -4306,7 +4298,7 @@
         <v>2.0</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
@@ -4315,7 +4307,7 @@
     </row>
     <row r="118">
       <c r="A118" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>8</v>
@@ -4324,7 +4316,7 @@
         <v>24</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E118" s="4">
         <v>270.0</v>
@@ -4333,7 +4325,7 @@
         <v>2.0</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
@@ -4342,7 +4334,7 @@
     </row>
     <row r="119">
       <c r="A119" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>8</v>
@@ -4351,7 +4343,7 @@
         <v>24</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E119" s="4">
         <v>375.0</v>
@@ -4360,7 +4352,7 @@
         <v>2.0</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
@@ -4369,7 +4361,7 @@
     </row>
     <row r="120">
       <c r="A120" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>8</v>
@@ -4378,7 +4370,7 @@
         <v>9</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E120" s="4">
         <v>375.0</v>
@@ -4387,7 +4379,7 @@
         <v>2.0</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
@@ -4396,7 +4388,7 @@
     </row>
     <row r="121">
       <c r="A121" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>8</v>
@@ -4405,7 +4397,7 @@
         <v>28</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E121" s="4">
         <v>375.0</v>
@@ -4414,7 +4406,7 @@
         <v>5.0</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
@@ -4423,16 +4415,16 @@
     </row>
     <row r="122">
       <c r="A122" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C122" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D122" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="E122" s="4">
         <v>375.0</v>
@@ -4441,7 +4433,7 @@
         <v>10</v>
       </c>
       <c r="G122" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
@@ -4450,16 +4442,16 @@
     </row>
     <row r="123">
       <c r="A123" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E123" s="4">
         <v>375.0</v>
@@ -4468,7 +4460,7 @@
         <v>10</v>
       </c>
       <c r="G123" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
@@ -4477,7 +4469,7 @@
     </row>
     <row r="124">
       <c r="A124" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>8</v>
@@ -4486,7 +4478,7 @@
         <v>32</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E124" s="4">
         <v>375.0</v>
@@ -4495,7 +4487,7 @@
         <v>5.0</v>
       </c>
       <c r="G124" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
@@ -4504,7 +4496,7 @@
     </row>
     <row r="125">
       <c r="A125" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>8</v>
@@ -4513,7 +4505,7 @@
         <v>9</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E125" s="4">
         <v>400.0</v>
@@ -4522,7 +4514,7 @@
         <v>2.0</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
@@ -4531,7 +4523,7 @@
     </row>
     <row r="126">
       <c r="A126" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>8</v>
@@ -4540,7 +4532,7 @@
         <v>9</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E126" s="4">
         <v>375.0</v>
@@ -4549,7 +4541,7 @@
         <v>2.0</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
@@ -4558,7 +4550,7 @@
     </row>
     <row r="127">
       <c r="A127" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>8</v>
@@ -4567,7 +4559,7 @@
         <v>28</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E127" s="4">
         <v>375.0</v>
@@ -4576,7 +4568,7 @@
         <v>6.0</v>
       </c>
       <c r="G127" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
@@ -4585,16 +4577,16 @@
     </row>
     <row r="128">
       <c r="A128" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C128" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="E128" s="4">
         <v>375.0</v>
@@ -4603,7 +4595,7 @@
         <v>10</v>
       </c>
       <c r="G128" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
@@ -4612,16 +4604,16 @@
     </row>
     <row r="129">
       <c r="A129" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E129" s="4">
         <v>375.0</v>
@@ -4630,7 +4622,7 @@
         <v>10</v>
       </c>
       <c r="G129" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
@@ -4639,7 +4631,7 @@
     </row>
     <row r="130">
       <c r="A130" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>20</v>
@@ -4648,7 +4640,7 @@
         <v>38</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E130" s="4">
         <v>600.0</v>
@@ -4657,7 +4649,7 @@
         <v>10</v>
       </c>
       <c r="G130" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
@@ -4666,7 +4658,7 @@
     </row>
     <row r="131">
       <c r="A131" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B131" s="8" t="s">
         <v>20</v>
@@ -4675,7 +4667,7 @@
         <v>9</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E131" s="4">
         <v>375.0</v>
@@ -4684,7 +4676,7 @@
         <v>2.0</v>
       </c>
       <c r="G131" s="4" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
@@ -4693,7 +4685,7 @@
     </row>
     <row r="132">
       <c r="A132" s="4" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B132" s="4" t="s">
         <v>8</v>
@@ -4702,7 +4694,7 @@
         <v>24</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E132" s="4">
         <v>425.0</v>
@@ -4711,7 +4703,7 @@
         <v>6.0</v>
       </c>
       <c r="G132" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
@@ -4720,16 +4712,16 @@
     </row>
     <row r="133">
       <c r="A133" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E133" s="4">
         <v>425.0</v>
@@ -4738,7 +4730,7 @@
         <v>3.0</v>
       </c>
       <c r="G133" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
@@ -4747,7 +4739,7 @@
     </row>
     <row r="134">
       <c r="A134" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>8</v>
@@ -4756,7 +4748,7 @@
         <v>24</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E134" s="4">
         <v>425.0</v>
@@ -4765,7 +4757,7 @@
         <v>3.0</v>
       </c>
       <c r="G134" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
@@ -4774,16 +4766,16 @@
     </row>
     <row r="135">
       <c r="A135" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B135" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E135" s="4">
         <v>425.0</v>
@@ -4792,7 +4784,7 @@
         <v>10</v>
       </c>
       <c r="G135" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
@@ -4801,7 +4793,7 @@
     </row>
     <row r="136">
       <c r="A136" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>8</v>
@@ -4810,7 +4802,7 @@
         <v>28</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E136" s="4">
         <v>425.0</v>
@@ -4819,7 +4811,7 @@
         <v>5.0</v>
       </c>
       <c r="G136" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
@@ -4828,7 +4820,7 @@
     </row>
     <row r="137">
       <c r="A137" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B137" s="4" t="s">
         <v>8</v>
@@ -4837,7 +4829,7 @@
         <v>9</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E137" s="4">
         <v>375.0</v>
@@ -4853,16 +4845,16 @@
     </row>
     <row r="138">
       <c r="A138" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B138" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E138" s="4">
         <v>425.0</v>
@@ -4871,7 +4863,7 @@
         <v>10</v>
       </c>
       <c r="G138" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H138" s="3"/>
       <c r="I138" s="3"/>
@@ -4880,7 +4872,7 @@
     </row>
     <row r="139">
       <c r="A139" s="4" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>20</v>
@@ -4889,7 +4881,7 @@
         <v>38</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E139" s="4">
         <v>1000.0</v>
@@ -4898,7 +4890,7 @@
         <v>10</v>
       </c>
       <c r="G139" s="4" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H139" s="3"/>
       <c r="I139" s="3"/>
@@ -4907,7 +4899,7 @@
     </row>
     <row r="140">
       <c r="A140" s="4" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B140" s="4" t="s">
         <v>20</v>
@@ -4916,7 +4908,7 @@
         <v>38</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E140" s="4">
         <v>150.0</v>
@@ -4925,7 +4917,7 @@
         <v>10</v>
       </c>
       <c r="G140" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H140" s="3"/>
       <c r="I140" s="3"/>
@@ -4934,7 +4926,7 @@
     </row>
     <row r="141">
       <c r="A141" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B141" s="4" t="s">
         <v>20</v>
@@ -4943,7 +4935,7 @@
         <v>32</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E141" s="4">
         <v>425.0</v>
@@ -4952,7 +4944,7 @@
         <v>6.0</v>
       </c>
       <c r="G141" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H141" s="3"/>
       <c r="I141" s="3"/>
@@ -4961,7 +4953,7 @@
     </row>
     <row r="142">
       <c r="A142" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>20</v>
@@ -4970,7 +4962,7 @@
         <v>32</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E142" s="4">
         <v>425.0</v>
@@ -4979,7 +4971,7 @@
         <v>7.0</v>
       </c>
       <c r="G142" s="4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="H142" s="3"/>
       <c r="I142" s="3"/>
@@ -4988,7 +4980,7 @@
     </row>
     <row r="143">
       <c r="A143" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B143" s="4" t="s">
         <v>8</v>
@@ -4997,7 +4989,7 @@
         <v>9</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E143" s="4">
         <v>400.0</v>
@@ -5006,7 +4998,7 @@
         <v>2.0</v>
       </c>
       <c r="G143" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H143" s="3"/>
       <c r="I143" s="3"/>
@@ -5015,7 +5007,7 @@
     </row>
     <row r="144">
       <c r="A144" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B144" s="4" t="s">
         <v>8</v>
@@ -5024,7 +5016,7 @@
         <v>28</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E144" s="4">
         <v>425.0</v>
@@ -5033,7 +5025,7 @@
         <v>5.0</v>
       </c>
       <c r="G144" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H144" s="3"/>
       <c r="I144" s="3"/>
@@ -5042,7 +5034,7 @@
     </row>
     <row r="145">
       <c r="A145" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B145" s="4" t="s">
         <v>12</v>
@@ -5051,7 +5043,7 @@
         <v>38</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E145" s="4">
         <v>750.0</v>
@@ -5060,7 +5052,7 @@
         <v>2.0</v>
       </c>
       <c r="G145" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
@@ -5069,7 +5061,7 @@
     </row>
     <row r="146">
       <c r="A146" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B146" s="4" t="s">
         <v>12</v>
@@ -5078,7 +5070,7 @@
         <v>38</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E146" s="4">
         <v>750.0</v>
@@ -5087,7 +5079,7 @@
         <v>2.0</v>
       </c>
       <c r="G146" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H146" s="3"/>
       <c r="I146" s="3"/>
@@ -5096,7 +5088,7 @@
     </row>
     <row r="147">
       <c r="A147" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>12</v>
@@ -5105,7 +5097,7 @@
         <v>38</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E147" s="4">
         <v>750.0</v>
@@ -5114,7 +5106,7 @@
         <v>2.0</v>
       </c>
       <c r="G147" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H147" s="3"/>
       <c r="I147" s="3"/>
@@ -5123,7 +5115,7 @@
     </row>
     <row r="148">
       <c r="A148" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>12</v>
@@ -5132,7 +5124,7 @@
         <v>38</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E148" s="4">
         <v>750.0</v>
@@ -5141,7 +5133,7 @@
         <v>2.0</v>
       </c>
       <c r="G148" s="4" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H148" s="3"/>
       <c r="I148" s="3"/>

</xml_diff>